<commit_message>
Update 24 January 2024 - Bug Absen dinas malam
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_JADWAL_NEW.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_JADWAL_NEW.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="42">
   <si>
     <t xml:space="preserve">KD_PGW</t>
   </si>
@@ -40,16 +40,112 @@
     <t xml:space="preserve">HARI_NASIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">000000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPV1</t>
+    <t xml:space="preserve">0323230002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
   </si>
   <si>
     <t xml:space="preserve">2024-02</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-02-01</t>
+    <t xml:space="preserve">2024-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-31</t>
   </si>
 </sst>
 </file>
@@ -189,13 +285,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.28"/>
@@ -226,7 +322,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -246,6 +342,607 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update 22 February 2024 - Bug Import shift schedule
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_JADWAL_NEW.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_JADWAL_NEW.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">HARI_NASIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">0323230002</t>
+    <t xml:space="preserve">0324240006</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
@@ -288,7 +288,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>